<commit_message>
Fix: corrigiendo errores de redacción
</commit_message>
<xml_diff>
--- a/5. Historias de usuario/Historias de Usuario Proyecto Legajo.xlsx
+++ b/5. Historias de usuario/Historias de Usuario Proyecto Legajo.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="aZIASUTpVKfNXjFNqBU6a/wYntUxj10/4WvPa415eIk="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="uk7Qm8/C2FIrEcWzDiZDhYW0yjGHhUV2E9He0TdY3pg="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="291">
   <si>
     <t>Enunciado de la historia</t>
   </si>
@@ -370,36 +370,6 @@
     <t>el sistema no registrará el libro y mostrara el mensaje "El libro ya se encuentra en el sistema"</t>
   </si>
   <si>
-    <t>2.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Necesito organizar los libros en el inventario con etiquetas </t>
-  </si>
-  <si>
-    <t>Con la finalidad de que los libros esten ordenados por diferentes categorias</t>
-  </si>
-  <si>
-    <t>El bibliotecario registra los libros con etiquetas</t>
-  </si>
-  <si>
-    <t>En caso que el bibliotecario agrege etiquetas al libro que esté editando o registrando</t>
-  </si>
-  <si>
-    <t>cuando el bibliotecario publica los cambios</t>
-  </si>
-  <si>
-    <t>el sistema mostrará el libro en sus categorías correspondientes según sus etiquetas</t>
-  </si>
-  <si>
-    <t>El bibliotecario no registra los libros con etiquetas</t>
-  </si>
-  <si>
-    <t>En caso que el bibliotecario no agrege etiquetas al libro que esté editando o registrando</t>
-  </si>
-  <si>
-    <t>el sistema mostrará el libro en la categoría "sin etiquetas"</t>
-  </si>
-  <si>
     <t>2.4</t>
   </si>
   <si>
@@ -551,7 +521,7 @@
     <t>Registrar una entrega de libro para un préstamo nuevo</t>
   </si>
   <si>
-    <t>El bibliotecario accede a la página para registrar una entrega, asegurándose de completar todos los detalles del préstamo</t>
+    <t>El bibliotecario accede al sistema para registrar una entrega, asegurándose de completar todos los detalles del préstamo</t>
   </si>
   <si>
     <t>El bibliotecario marca el libro como entregado al usuario</t>
@@ -572,7 +542,7 @@
     <t>Registrar un retraso en la devolución</t>
   </si>
   <si>
-    <t>El bibliotecario accede a la página de "Gestionar Retrasos" para registrar un retraso en un libro no devuelto a tiempo</t>
+    <t>El bibliotecario accede a la sección de "Gestionar Retrasos" para registrar un retraso en un libro no devuelto a tiempo</t>
   </si>
   <si>
     <t>El bibliotecario introduce un retraso en un libro que no ha sido devuelto en la fecha esperada</t>
@@ -739,7 +709,7 @@
     <t>El usuario selecciona un evento.</t>
   </si>
   <si>
-    <t>El sistema muestra la página solo de ese evento en especifico.</t>
+    <t>El sistema muestra la descripción solo de ese evento en especifico.</t>
   </si>
   <si>
     <t>5.1.1</t>
@@ -754,7 +724,7 @@
     <t>El sistema muestra todos los detalles del evento seleccionado.</t>
   </si>
   <si>
-    <t>El sistema muestra una página detallada del evento.</t>
+    <t>El sistema muestra una descripción detallada del evento.</t>
   </si>
   <si>
     <t>El usuario selecciona un evento para ver más detalles.</t>
@@ -3310,7 +3280,7 @@
       <c r="Y54" s="1"/>
       <c r="Z54" s="1"/>
     </row>
-    <row r="55" ht="29.25" customHeight="1">
+    <row r="55" ht="30.0" customHeight="1">
       <c r="A55" s="1"/>
       <c r="B55" s="13"/>
       <c r="C55" s="13"/>
@@ -3326,10 +3296,10 @@
         <v>125</v>
       </c>
       <c r="I55" s="10" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
@@ -3435,31 +3405,31 @@
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="1"/>
       <c r="B59" s="9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C59" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F59" s="20">
         <v>1.0</v>
       </c>
       <c r="G59" s="21" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H59" s="21" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I59" s="21" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J59" s="21" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
@@ -3478,7 +3448,7 @@
       <c r="Y59" s="1"/>
       <c r="Z59" s="1"/>
     </row>
-    <row r="60" ht="30.0" customHeight="1">
+    <row r="60" ht="44.25" customHeight="1">
       <c r="A60" s="1"/>
       <c r="B60" s="13"/>
       <c r="C60" s="13"/>
@@ -3488,13 +3458,13 @@
         <v>2.0</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H60" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I60" s="10" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="J60" s="10" t="s">
         <v>137</v>
@@ -3646,7 +3616,7 @@
       <c r="Y64" s="1"/>
       <c r="Z64" s="1"/>
     </row>
-    <row r="65" ht="44.25" customHeight="1">
+    <row r="65" ht="45.75" customHeight="1">
       <c r="A65" s="1"/>
       <c r="B65" s="13"/>
       <c r="C65" s="13"/>
@@ -3662,10 +3632,10 @@
         <v>146</v>
       </c>
       <c r="I65" s="10" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="J65" s="10" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
@@ -3771,31 +3741,31 @@
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="1"/>
       <c r="B69" s="9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C69" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D69" s="10" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E69" s="10" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F69" s="20">
         <v>1.0</v>
       </c>
       <c r="G69" s="21" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H69" s="21" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I69" s="21" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J69" s="21" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K69" s="1"/>
       <c r="L69" s="1"/>
@@ -3814,7 +3784,7 @@
       <c r="Y69" s="1"/>
       <c r="Z69" s="1"/>
     </row>
-    <row r="70" ht="45.75" customHeight="1">
+    <row r="70" ht="42.75" customHeight="1">
       <c r="A70" s="1"/>
       <c r="B70" s="13"/>
       <c r="C70" s="13"/>
@@ -3824,13 +3794,13 @@
         <v>2.0</v>
       </c>
       <c r="G70" s="10" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H70" s="10" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I70" s="10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J70" s="10" t="s">
         <v>158</v>
@@ -3982,7 +3952,7 @@
       <c r="Y74" s="1"/>
       <c r="Z74" s="1"/>
     </row>
-    <row r="75" ht="42.75" customHeight="1">
+    <row r="75" ht="28.5" customHeight="1">
       <c r="A75" s="1"/>
       <c r="B75" s="13"/>
       <c r="C75" s="13"/>
@@ -3998,10 +3968,10 @@
         <v>167</v>
       </c>
       <c r="I75" s="10" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="J75" s="10" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="K75" s="1"/>
       <c r="L75" s="1"/>
@@ -4083,7 +4053,7 @@
       <c r="D78" s="19"/>
       <c r="E78" s="19"/>
       <c r="F78" s="18"/>
-      <c r="G78" s="19"/>
+      <c r="G78" s="24"/>
       <c r="H78" s="19"/>
       <c r="I78" s="19"/>
       <c r="J78" s="19"/>
@@ -4107,33 +4077,33 @@
     <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="1"/>
       <c r="B79" s="9" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C79" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D79" s="10" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E79" s="10" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F79" s="20">
         <v>1.0</v>
       </c>
       <c r="G79" s="21" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H79" s="21" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I79" s="21" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J79" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="K79" s="1"/>
+        <v>176</v>
+      </c>
+      <c r="K79" s="25"/>
       <c r="L79" s="1"/>
       <c r="M79" s="1"/>
       <c r="N79" s="1"/>
@@ -4150,7 +4120,7 @@
       <c r="Y79" s="1"/>
       <c r="Z79" s="1"/>
     </row>
-    <row r="80" ht="28.5" customHeight="1">
+    <row r="80" ht="51.75" customHeight="1">
       <c r="A80" s="1"/>
       <c r="B80" s="13"/>
       <c r="C80" s="13"/>
@@ -4160,18 +4130,18 @@
         <v>2.0</v>
       </c>
       <c r="G80" s="10" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H80" s="10" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I80" s="10" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J80" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="K80" s="1"/>
+        <v>180</v>
+      </c>
+      <c r="K80" s="25"/>
       <c r="L80" s="1"/>
       <c r="M80" s="1"/>
       <c r="N80" s="1"/>
@@ -4199,7 +4169,7 @@
       <c r="H81" s="13"/>
       <c r="I81" s="13"/>
       <c r="J81" s="13"/>
-      <c r="K81" s="1"/>
+      <c r="K81" s="25"/>
       <c r="L81" s="1"/>
       <c r="M81" s="1"/>
       <c r="N81" s="1"/>
@@ -4227,7 +4197,7 @@
       <c r="H82" s="14"/>
       <c r="I82" s="14"/>
       <c r="J82" s="14"/>
-      <c r="K82" s="1"/>
+      <c r="K82" s="25"/>
       <c r="L82" s="1"/>
       <c r="M82" s="1"/>
       <c r="N82" s="1"/>
@@ -4251,7 +4221,7 @@
       <c r="D83" s="19"/>
       <c r="E83" s="19"/>
       <c r="F83" s="18"/>
-      <c r="G83" s="24"/>
+      <c r="G83" s="19"/>
       <c r="H83" s="19"/>
       <c r="I83" s="19"/>
       <c r="J83" s="19"/>
@@ -4273,35 +4243,35 @@
       <c r="Z83" s="1"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="1"/>
+      <c r="A84" s="26"/>
       <c r="B84" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C84" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D84" s="10" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E84" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="F84" s="20">
+        <v>183</v>
+      </c>
+      <c r="F84" s="12">
         <v>1.0</v>
       </c>
-      <c r="G84" s="21" t="s">
-        <v>183</v>
-      </c>
-      <c r="H84" s="21" t="s">
+      <c r="G84" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="I84" s="21" t="s">
+      <c r="H84" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="J84" s="21" t="s">
+      <c r="I84" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="K84" s="25"/>
+      <c r="J84" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="K84" s="1"/>
       <c r="L84" s="1"/>
       <c r="M84" s="1"/>
       <c r="N84" s="1"/>
@@ -4318,28 +4288,18 @@
       <c r="Y84" s="1"/>
       <c r="Z84" s="1"/>
     </row>
-    <row r="85" ht="51.75" customHeight="1">
-      <c r="A85" s="1"/>
+    <row r="85" ht="15.75" customHeight="1">
+      <c r="A85" s="26"/>
       <c r="B85" s="13"/>
       <c r="C85" s="13"/>
       <c r="D85" s="13"/>
       <c r="E85" s="13"/>
-      <c r="F85" s="12">
-        <v>2.0</v>
-      </c>
-      <c r="G85" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="H85" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="I85" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="J85" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="K85" s="25"/>
+      <c r="F85" s="13"/>
+      <c r="G85" s="13"/>
+      <c r="H85" s="13"/>
+      <c r="I85" s="13"/>
+      <c r="J85" s="13"/>
+      <c r="K85" s="1"/>
       <c r="L85" s="1"/>
       <c r="M85" s="1"/>
       <c r="N85" s="1"/>
@@ -4357,7 +4317,7 @@
       <c r="Z85" s="1"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="1"/>
+      <c r="A86" s="26"/>
       <c r="B86" s="13"/>
       <c r="C86" s="13"/>
       <c r="D86" s="13"/>
@@ -4367,7 +4327,7 @@
       <c r="H86" s="13"/>
       <c r="I86" s="13"/>
       <c r="J86" s="13"/>
-      <c r="K86" s="25"/>
+      <c r="K86" s="1"/>
       <c r="L86" s="1"/>
       <c r="M86" s="1"/>
       <c r="N86" s="1"/>
@@ -4385,7 +4345,7 @@
       <c r="Z86" s="1"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="1"/>
+      <c r="A87" s="26"/>
       <c r="B87" s="14"/>
       <c r="C87" s="14"/>
       <c r="D87" s="14"/>
@@ -4395,7 +4355,7 @@
       <c r="H87" s="14"/>
       <c r="I87" s="14"/>
       <c r="J87" s="14"/>
-      <c r="K87" s="25"/>
+      <c r="K87" s="1"/>
       <c r="L87" s="1"/>
       <c r="M87" s="1"/>
       <c r="N87" s="1"/>
@@ -4441,33 +4401,33 @@
       <c r="Z88" s="1"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="26"/>
+      <c r="A89" s="1"/>
       <c r="B89" s="9" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C89" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D89" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="E89" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="F89" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="G89" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="H89" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="E89" s="10" t="s">
+      <c r="I89" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="F89" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="G89" s="10" t="s">
+      <c r="J89" s="21" t="s">
         <v>194</v>
-      </c>
-      <c r="H89" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="I89" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="J89" s="10" t="s">
-        <v>197</v>
       </c>
       <c r="K89" s="1"/>
       <c r="L89" s="1"/>
@@ -4486,17 +4446,27 @@
       <c r="Y89" s="1"/>
       <c r="Z89" s="1"/>
     </row>
-    <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="26"/>
+    <row r="90" ht="33.0" customHeight="1">
+      <c r="A90" s="1"/>
       <c r="B90" s="13"/>
       <c r="C90" s="13"/>
       <c r="D90" s="13"/>
       <c r="E90" s="13"/>
-      <c r="F90" s="13"/>
-      <c r="G90" s="13"/>
-      <c r="H90" s="13"/>
-      <c r="I90" s="13"/>
-      <c r="J90" s="13"/>
+      <c r="F90" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="G90" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="H90" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="I90" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="J90" s="10" t="s">
+        <v>197</v>
+      </c>
       <c r="K90" s="1"/>
       <c r="L90" s="1"/>
       <c r="M90" s="1"/>
@@ -4515,7 +4485,7 @@
       <c r="Z90" s="1"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="26"/>
+      <c r="A91" s="1"/>
       <c r="B91" s="13"/>
       <c r="C91" s="13"/>
       <c r="D91" s="13"/>
@@ -4543,7 +4513,7 @@
       <c r="Z91" s="1"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="26"/>
+      <c r="A92" s="1"/>
       <c r="B92" s="14"/>
       <c r="C92" s="14"/>
       <c r="D92" s="14"/>
@@ -4612,19 +4582,19 @@
       <c r="E94" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="F94" s="20">
+      <c r="F94" s="12">
         <v>1.0</v>
       </c>
-      <c r="G94" s="21" t="s">
+      <c r="G94" s="27" t="s">
         <v>201</v>
       </c>
-      <c r="H94" s="21" t="s">
+      <c r="H94" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="I94" s="21" t="s">
+      <c r="I94" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="J94" s="21" t="s">
+      <c r="J94" s="10" t="s">
         <v>204</v>
       </c>
       <c r="K94" s="1"/>
@@ -4644,27 +4614,17 @@
       <c r="Y94" s="1"/>
       <c r="Z94" s="1"/>
     </row>
-    <row r="95" ht="33.0" customHeight="1">
+    <row r="95" ht="15.75" customHeight="1">
       <c r="A95" s="1"/>
       <c r="B95" s="13"/>
       <c r="C95" s="13"/>
       <c r="D95" s="13"/>
       <c r="E95" s="13"/>
-      <c r="F95" s="12">
-        <v>2.0</v>
-      </c>
-      <c r="G95" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="H95" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="I95" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="J95" s="10" t="s">
-        <v>207</v>
-      </c>
+      <c r="F95" s="13"/>
+      <c r="G95" s="28"/>
+      <c r="H95" s="13"/>
+      <c r="I95" s="13"/>
+      <c r="J95" s="13"/>
       <c r="K95" s="1"/>
       <c r="L95" s="1"/>
       <c r="M95" s="1"/>
@@ -4689,7 +4649,7 @@
       <c r="D96" s="13"/>
       <c r="E96" s="13"/>
       <c r="F96" s="13"/>
-      <c r="G96" s="13"/>
+      <c r="G96" s="28"/>
       <c r="H96" s="13"/>
       <c r="I96" s="13"/>
       <c r="J96" s="13"/>
@@ -4717,7 +4677,7 @@
       <c r="D97" s="14"/>
       <c r="E97" s="14"/>
       <c r="F97" s="14"/>
-      <c r="G97" s="14"/>
+      <c r="G97" s="29"/>
       <c r="H97" s="14"/>
       <c r="I97" s="14"/>
       <c r="J97" s="14"/>
@@ -4769,31 +4729,31 @@
     <row r="99" ht="15.75" customHeight="1">
       <c r="A99" s="1"/>
       <c r="B99" s="9" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C99" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D99" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="E99" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="F99" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="G99" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="H99" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="E99" s="10" t="s">
+      <c r="I99" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="F99" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="G99" s="27" t="s">
+      <c r="J99" s="21" t="s">
         <v>211</v>
-      </c>
-      <c r="H99" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="I99" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="J99" s="10" t="s">
-        <v>214</v>
       </c>
       <c r="K99" s="1"/>
       <c r="L99" s="1"/>
@@ -4812,17 +4772,27 @@
       <c r="Y99" s="1"/>
       <c r="Z99" s="1"/>
     </row>
-    <row r="100" ht="15.75" customHeight="1">
+    <row r="100" ht="39.75" customHeight="1">
       <c r="A100" s="1"/>
       <c r="B100" s="13"/>
       <c r="C100" s="13"/>
       <c r="D100" s="13"/>
       <c r="E100" s="13"/>
-      <c r="F100" s="13"/>
-      <c r="G100" s="28"/>
-      <c r="H100" s="13"/>
-      <c r="I100" s="13"/>
-      <c r="J100" s="13"/>
+      <c r="F100" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="G100" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="H100" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="I100" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="J100" s="10" t="s">
+        <v>215</v>
+      </c>
       <c r="K100" s="1"/>
       <c r="L100" s="1"/>
       <c r="M100" s="1"/>
@@ -4847,7 +4817,7 @@
       <c r="D101" s="13"/>
       <c r="E101" s="13"/>
       <c r="F101" s="13"/>
-      <c r="G101" s="28"/>
+      <c r="G101" s="13"/>
       <c r="H101" s="13"/>
       <c r="I101" s="13"/>
       <c r="J101" s="13"/>
@@ -4875,7 +4845,7 @@
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
       <c r="F102" s="14"/>
-      <c r="G102" s="29"/>
+      <c r="G102" s="14"/>
       <c r="H102" s="14"/>
       <c r="I102" s="14"/>
       <c r="J102" s="14"/>
@@ -4927,31 +4897,31 @@
     <row r="104" ht="15.75" customHeight="1">
       <c r="A104" s="1"/>
       <c r="B104" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C104" s="10" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D104" s="10" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E104" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="F104" s="20">
+        <v>218</v>
+      </c>
+      <c r="F104" s="12">
         <v>1.0</v>
       </c>
-      <c r="G104" s="21" t="s">
-        <v>218</v>
-      </c>
-      <c r="H104" s="21" t="s">
+      <c r="G104" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="I104" s="21" t="s">
+      <c r="H104" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="J104" s="21" t="s">
+      <c r="I104" s="10" t="s">
         <v>221</v>
+      </c>
+      <c r="J104" s="10" t="s">
+        <v>222</v>
       </c>
       <c r="K104" s="1"/>
       <c r="L104" s="1"/>
@@ -4970,27 +4940,17 @@
       <c r="Y104" s="1"/>
       <c r="Z104" s="1"/>
     </row>
-    <row r="105" ht="39.75" customHeight="1">
+    <row r="105" ht="15.75" customHeight="1">
       <c r="A105" s="1"/>
       <c r="B105" s="13"/>
       <c r="C105" s="13"/>
       <c r="D105" s="13"/>
       <c r="E105" s="13"/>
-      <c r="F105" s="12">
-        <v>2.0</v>
-      </c>
-      <c r="G105" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="H105" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="I105" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="J105" s="10" t="s">
-        <v>225</v>
-      </c>
+      <c r="F105" s="13"/>
+      <c r="G105" s="13"/>
+      <c r="H105" s="13"/>
+      <c r="I105" s="13"/>
+      <c r="J105" s="13"/>
       <c r="K105" s="1"/>
       <c r="L105" s="1"/>
       <c r="M105" s="1"/>
@@ -5095,31 +5055,31 @@
     <row r="109" ht="15.75" customHeight="1">
       <c r="A109" s="1"/>
       <c r="B109" s="9" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C109" s="10" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D109" s="10" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E109" s="10" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F109" s="12">
         <v>1.0</v>
       </c>
       <c r="G109" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="H109" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="I109" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="J109" s="10" t="s">
         <v>229</v>
-      </c>
-      <c r="H109" s="10" t="s">
-        <v>230</v>
-      </c>
-      <c r="I109" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="J109" s="10" t="s">
-        <v>232</v>
       </c>
       <c r="K109" s="1"/>
       <c r="L109" s="1"/>
@@ -5253,31 +5213,31 @@
     <row r="114" ht="15.75" customHeight="1">
       <c r="A114" s="1"/>
       <c r="B114" s="9" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C114" s="10" t="s">
         <v>90</v>
       </c>
       <c r="D114" s="10" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E114" s="10" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F114" s="12">
         <v>1.0</v>
       </c>
       <c r="G114" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="H114" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="I114" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="J114" s="10" t="s">
         <v>236</v>
-      </c>
-      <c r="H114" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="I114" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="J114" s="10" t="s">
-        <v>239</v>
       </c>
       <c r="K114" s="1"/>
       <c r="L114" s="1"/>
@@ -5411,31 +5371,31 @@
     <row r="119" ht="15.75" customHeight="1">
       <c r="A119" s="1"/>
       <c r="B119" s="9" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C119" s="10" t="s">
         <v>90</v>
       </c>
       <c r="D119" s="10" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E119" s="10" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="F119" s="12">
         <v>1.0</v>
       </c>
       <c r="G119" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="H119" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="I119" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="J119" s="10" t="s">
         <v>243</v>
-      </c>
-      <c r="H119" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="I119" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="J119" s="10" t="s">
-        <v>246</v>
       </c>
       <c r="K119" s="1"/>
       <c r="L119" s="1"/>
@@ -5569,31 +5529,31 @@
     <row r="124" ht="15.75" customHeight="1">
       <c r="A124" s="1"/>
       <c r="B124" s="9" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C124" s="10" t="s">
         <v>90</v>
       </c>
       <c r="D124" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="E124" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="F124" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="G124" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="H124" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="E124" s="10" t="s">
+      <c r="I124" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="F124" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="G124" s="10" t="s">
+      <c r="J124" s="21" t="s">
         <v>250</v>
-      </c>
-      <c r="H124" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="I124" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="J124" s="10" t="s">
-        <v>253</v>
       </c>
       <c r="K124" s="1"/>
       <c r="L124" s="1"/>
@@ -5612,17 +5572,27 @@
       <c r="Y124" s="1"/>
       <c r="Z124" s="1"/>
     </row>
-    <row r="125" ht="15.75" customHeight="1">
+    <row r="125" ht="42.0" customHeight="1">
       <c r="A125" s="1"/>
       <c r="B125" s="13"/>
       <c r="C125" s="13"/>
       <c r="D125" s="13"/>
       <c r="E125" s="13"/>
-      <c r="F125" s="13"/>
-      <c r="G125" s="13"/>
-      <c r="H125" s="13"/>
-      <c r="I125" s="13"/>
-      <c r="J125" s="13"/>
+      <c r="F125" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="G125" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="H125" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="I125" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="J125" s="10" t="s">
+        <v>254</v>
+      </c>
       <c r="K125" s="1"/>
       <c r="L125" s="1"/>
       <c r="M125" s="1"/>
@@ -5727,31 +5697,31 @@
     <row r="129" ht="15.75" customHeight="1">
       <c r="A129" s="1"/>
       <c r="B129" s="9" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C129" s="10" t="s">
         <v>90</v>
       </c>
       <c r="D129" s="10" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E129" s="10" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F129" s="20">
         <v>1.0</v>
       </c>
       <c r="G129" s="21" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H129" s="21" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="I129" s="21" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="J129" s="21" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="K129" s="1"/>
       <c r="L129" s="1"/>
@@ -5770,7 +5740,7 @@
       <c r="Y129" s="1"/>
       <c r="Z129" s="1"/>
     </row>
-    <row r="130" ht="42.0" customHeight="1">
+    <row r="130" ht="66.0" customHeight="1">
       <c r="A130" s="1"/>
       <c r="B130" s="13"/>
       <c r="C130" s="13"/>
@@ -5780,16 +5750,16 @@
         <v>2.0</v>
       </c>
       <c r="G130" s="10" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H130" s="10" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I130" s="10" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="J130" s="10" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="K130" s="1"/>
       <c r="L130" s="1"/>
@@ -5893,33 +5863,33 @@
       <c r="Z133" s="1"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="A134" s="1"/>
+      <c r="A134" s="26"/>
       <c r="B134" s="9" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C134" s="10" t="s">
         <v>90</v>
       </c>
       <c r="D134" s="10" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E134" s="10" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="F134" s="20">
         <v>1.0</v>
       </c>
       <c r="G134" s="21" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="H134" s="21" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="I134" s="21" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="J134" s="21" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="K134" s="1"/>
       <c r="L134" s="1"/>
@@ -5938,8 +5908,8 @@
       <c r="Y134" s="1"/>
       <c r="Z134" s="1"/>
     </row>
-    <row r="135" ht="66.0" customHeight="1">
-      <c r="A135" s="1"/>
+    <row r="135" ht="42.0" customHeight="1">
+      <c r="A135" s="26"/>
       <c r="B135" s="13"/>
       <c r="C135" s="13"/>
       <c r="D135" s="13"/>
@@ -5948,16 +5918,16 @@
         <v>2.0</v>
       </c>
       <c r="G135" s="10" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="H135" s="10" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="I135" s="10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="J135" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="K135" s="1"/>
       <c r="L135" s="1"/>
@@ -5977,7 +5947,7 @@
       <c r="Z135" s="1"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="A136" s="1"/>
+      <c r="A136" s="26"/>
       <c r="B136" s="13"/>
       <c r="C136" s="13"/>
       <c r="D136" s="13"/>
@@ -6005,7 +5975,7 @@
       <c r="Z136" s="1"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="A137" s="1"/>
+      <c r="A137" s="26"/>
       <c r="B137" s="14"/>
       <c r="C137" s="14"/>
       <c r="D137" s="14"/>
@@ -6061,33 +6031,33 @@
       <c r="Z138" s="1"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="A139" s="26"/>
+      <c r="A139" s="1"/>
       <c r="B139" s="9" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C139" s="10" t="s">
         <v>90</v>
       </c>
       <c r="D139" s="10" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E139" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="F139" s="20">
+        <v>279</v>
+      </c>
+      <c r="F139" s="12">
         <v>1.0</v>
       </c>
-      <c r="G139" s="21" t="s">
-        <v>279</v>
-      </c>
-      <c r="H139" s="21" t="s">
+      <c r="G139" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="I139" s="21" t="s">
+      <c r="H139" s="10" t="s">
         <v>281</v>
       </c>
-      <c r="J139" s="21" t="s">
+      <c r="I139" s="10" t="s">
         <v>282</v>
+      </c>
+      <c r="J139" s="10" t="s">
+        <v>283</v>
       </c>
       <c r="K139" s="1"/>
       <c r="L139" s="1"/>
@@ -6106,27 +6076,17 @@
       <c r="Y139" s="1"/>
       <c r="Z139" s="1"/>
     </row>
-    <row r="140" ht="42.0" customHeight="1">
-      <c r="A140" s="26"/>
+    <row r="140" ht="15.75" customHeight="1">
+      <c r="A140" s="1"/>
       <c r="B140" s="13"/>
       <c r="C140" s="13"/>
       <c r="D140" s="13"/>
       <c r="E140" s="13"/>
-      <c r="F140" s="12">
-        <v>2.0</v>
-      </c>
-      <c r="G140" s="10" t="s">
-        <v>283</v>
-      </c>
-      <c r="H140" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="I140" s="10" t="s">
-        <v>285</v>
-      </c>
-      <c r="J140" s="10" t="s">
-        <v>286</v>
-      </c>
+      <c r="F140" s="13"/>
+      <c r="G140" s="13"/>
+      <c r="H140" s="13"/>
+      <c r="I140" s="13"/>
+      <c r="J140" s="13"/>
       <c r="K140" s="1"/>
       <c r="L140" s="1"/>
       <c r="M140" s="1"/>
@@ -6145,7 +6105,7 @@
       <c r="Z140" s="1"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="A141" s="26"/>
+      <c r="A141" s="1"/>
       <c r="B141" s="13"/>
       <c r="C141" s="13"/>
       <c r="D141" s="13"/>
@@ -6173,7 +6133,7 @@
       <c r="Z141" s="1"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="A142" s="26"/>
+      <c r="A142" s="1"/>
       <c r="B142" s="14"/>
       <c r="C142" s="14"/>
       <c r="D142" s="14"/>
@@ -6228,36 +6188,36 @@
       <c r="Y143" s="1"/>
       <c r="Z143" s="1"/>
     </row>
-    <row r="144" ht="15.75" customHeight="1">
-      <c r="A144" s="1"/>
+    <row r="144" ht="39.75" customHeight="1">
+      <c r="A144" s="26"/>
       <c r="B144" s="9" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C144" s="10" t="s">
         <v>90</v>
       </c>
       <c r="D144" s="10" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="E144" s="10" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="F144" s="12">
         <v>1.0</v>
       </c>
       <c r="G144" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="H144" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="I144" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="J144" s="10" t="s">
         <v>290</v>
       </c>
-      <c r="H144" s="10" t="s">
-        <v>291</v>
-      </c>
-      <c r="I144" s="10" t="s">
-        <v>292</v>
-      </c>
-      <c r="J144" s="10" t="s">
-        <v>293</v>
-      </c>
-      <c r="K144" s="1"/>
+      <c r="K144" s="25"/>
       <c r="L144" s="1"/>
       <c r="M144" s="1"/>
       <c r="N144" s="1"/>
@@ -6275,7 +6235,7 @@
       <c r="Z144" s="1"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="A145" s="1"/>
+      <c r="A145" s="26"/>
       <c r="B145" s="13"/>
       <c r="C145" s="13"/>
       <c r="D145" s="13"/>
@@ -6285,7 +6245,7 @@
       <c r="H145" s="13"/>
       <c r="I145" s="13"/>
       <c r="J145" s="13"/>
-      <c r="K145" s="1"/>
+      <c r="K145" s="25"/>
       <c r="L145" s="1"/>
       <c r="M145" s="1"/>
       <c r="N145" s="1"/>
@@ -6303,7 +6263,7 @@
       <c r="Z145" s="1"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="A146" s="1"/>
+      <c r="A146" s="26"/>
       <c r="B146" s="13"/>
       <c r="C146" s="13"/>
       <c r="D146" s="13"/>
@@ -6313,7 +6273,7 @@
       <c r="H146" s="13"/>
       <c r="I146" s="13"/>
       <c r="J146" s="13"/>
-      <c r="K146" s="1"/>
+      <c r="K146" s="25"/>
       <c r="L146" s="1"/>
       <c r="M146" s="1"/>
       <c r="N146" s="1"/>
@@ -6331,7 +6291,7 @@
       <c r="Z146" s="1"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="A147" s="1"/>
+      <c r="A147" s="26"/>
       <c r="B147" s="14"/>
       <c r="C147" s="14"/>
       <c r="D147" s="14"/>
@@ -6341,7 +6301,7 @@
       <c r="H147" s="14"/>
       <c r="I147" s="14"/>
       <c r="J147" s="14"/>
-      <c r="K147" s="1"/>
+      <c r="K147" s="25"/>
       <c r="L147" s="1"/>
       <c r="M147" s="1"/>
       <c r="N147" s="1"/>
@@ -6359,7 +6319,7 @@
       <c r="Z147" s="1"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="A148" s="1"/>
+      <c r="A148" s="26"/>
       <c r="B148" s="22"/>
       <c r="C148" s="19"/>
       <c r="D148" s="19"/>
@@ -6369,7 +6329,7 @@
       <c r="H148" s="19"/>
       <c r="I148" s="19"/>
       <c r="J148" s="19"/>
-      <c r="K148" s="1"/>
+      <c r="K148" s="25"/>
       <c r="L148" s="1"/>
       <c r="M148" s="1"/>
       <c r="N148" s="1"/>
@@ -6386,35 +6346,17 @@
       <c r="Y148" s="1"/>
       <c r="Z148" s="1"/>
     </row>
-    <row r="149" ht="39.75" customHeight="1">
+    <row r="149" ht="15.75" customHeight="1">
       <c r="A149" s="26"/>
-      <c r="B149" s="9" t="s">
-        <v>294</v>
-      </c>
-      <c r="C149" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D149" s="10" t="s">
-        <v>295</v>
-      </c>
-      <c r="E149" s="10" t="s">
-        <v>296</v>
-      </c>
-      <c r="F149" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="G149" s="10" t="s">
-        <v>297</v>
-      </c>
-      <c r="H149" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="I149" s="10" t="s">
-        <v>299</v>
-      </c>
-      <c r="J149" s="10" t="s">
-        <v>300</v>
-      </c>
+      <c r="B149" s="30"/>
+      <c r="C149" s="31"/>
+      <c r="D149" s="31"/>
+      <c r="E149" s="31"/>
+      <c r="F149" s="32"/>
+      <c r="G149" s="33"/>
+      <c r="H149" s="33"/>
+      <c r="I149" s="33"/>
+      <c r="J149" s="33"/>
       <c r="K149" s="25"/>
       <c r="L149" s="1"/>
       <c r="M149" s="1"/>
@@ -6434,15 +6376,15 @@
     </row>
     <row r="150" ht="15.75" customHeight="1">
       <c r="A150" s="26"/>
-      <c r="B150" s="13"/>
-      <c r="C150" s="13"/>
-      <c r="D150" s="13"/>
-      <c r="E150" s="13"/>
-      <c r="F150" s="13"/>
-      <c r="G150" s="13"/>
-      <c r="H150" s="13"/>
-      <c r="I150" s="13"/>
-      <c r="J150" s="13"/>
+      <c r="B150" s="34"/>
+      <c r="C150" s="34"/>
+      <c r="D150" s="34"/>
+      <c r="E150" s="34"/>
+      <c r="F150" s="35"/>
+      <c r="G150" s="36"/>
+      <c r="H150" s="36"/>
+      <c r="I150" s="36"/>
+      <c r="J150" s="36"/>
       <c r="K150" s="25"/>
       <c r="L150" s="1"/>
       <c r="M150" s="1"/>
@@ -6462,15 +6404,15 @@
     </row>
     <row r="151" ht="15.75" customHeight="1">
       <c r="A151" s="26"/>
-      <c r="B151" s="13"/>
-      <c r="C151" s="13"/>
-      <c r="D151" s="13"/>
-      <c r="E151" s="13"/>
-      <c r="F151" s="13"/>
-      <c r="G151" s="13"/>
-      <c r="H151" s="13"/>
-      <c r="I151" s="13"/>
-      <c r="J151" s="13"/>
+      <c r="B151" s="34"/>
+      <c r="C151" s="34"/>
+      <c r="D151" s="34"/>
+      <c r="E151" s="34"/>
+      <c r="F151" s="35"/>
+      <c r="G151" s="36"/>
+      <c r="H151" s="36"/>
+      <c r="I151" s="36"/>
+      <c r="J151" s="36"/>
       <c r="K151" s="25"/>
       <c r="L151" s="1"/>
       <c r="M151" s="1"/>
@@ -6490,15 +6432,15 @@
     </row>
     <row r="152" ht="15.75" customHeight="1">
       <c r="A152" s="26"/>
-      <c r="B152" s="14"/>
-      <c r="C152" s="14"/>
-      <c r="D152" s="14"/>
-      <c r="E152" s="14"/>
-      <c r="F152" s="14"/>
-      <c r="G152" s="14"/>
-      <c r="H152" s="14"/>
-      <c r="I152" s="14"/>
-      <c r="J152" s="14"/>
+      <c r="B152" s="37"/>
+      <c r="C152" s="37"/>
+      <c r="D152" s="37"/>
+      <c r="E152" s="37"/>
+      <c r="F152" s="35"/>
+      <c r="G152" s="36"/>
+      <c r="H152" s="36"/>
+      <c r="I152" s="36"/>
+      <c r="J152" s="36"/>
       <c r="K152" s="25"/>
       <c r="L152" s="1"/>
       <c r="M152" s="1"/>
@@ -6518,15 +6460,15 @@
     </row>
     <row r="153" ht="15.75" customHeight="1">
       <c r="A153" s="26"/>
-      <c r="B153" s="22"/>
-      <c r="C153" s="19"/>
-      <c r="D153" s="19"/>
-      <c r="E153" s="19"/>
-      <c r="F153" s="18"/>
-      <c r="G153" s="19"/>
-      <c r="H153" s="19"/>
-      <c r="I153" s="19"/>
-      <c r="J153" s="19"/>
+      <c r="B153" s="38"/>
+      <c r="C153" s="36"/>
+      <c r="D153" s="36"/>
+      <c r="E153" s="36"/>
+      <c r="F153" s="35"/>
+      <c r="G153" s="36"/>
+      <c r="H153" s="36"/>
+      <c r="I153" s="36"/>
+      <c r="J153" s="36"/>
       <c r="K153" s="25"/>
       <c r="L153" s="1"/>
       <c r="M153" s="1"/>
@@ -6545,17 +6487,17 @@
       <c r="Z153" s="1"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="A154" s="26"/>
-      <c r="B154" s="30"/>
-      <c r="C154" s="31"/>
-      <c r="D154" s="31"/>
-      <c r="E154" s="31"/>
-      <c r="F154" s="32"/>
-      <c r="G154" s="33"/>
-      <c r="H154" s="33"/>
-      <c r="I154" s="33"/>
-      <c r="J154" s="33"/>
-      <c r="K154" s="25"/>
+      <c r="A154" s="1"/>
+      <c r="B154" s="39"/>
+      <c r="C154" s="40"/>
+      <c r="D154" s="40"/>
+      <c r="E154" s="40"/>
+      <c r="F154" s="40"/>
+      <c r="G154" s="40"/>
+      <c r="H154" s="40"/>
+      <c r="I154" s="40"/>
+      <c r="J154" s="40"/>
+      <c r="K154" s="1"/>
       <c r="L154" s="1"/>
       <c r="M154" s="1"/>
       <c r="N154" s="1"/>
@@ -6573,17 +6515,17 @@
       <c r="Z154" s="1"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="A155" s="26"/>
-      <c r="B155" s="34"/>
-      <c r="C155" s="34"/>
-      <c r="D155" s="34"/>
-      <c r="E155" s="34"/>
-      <c r="F155" s="35"/>
-      <c r="G155" s="36"/>
-      <c r="H155" s="36"/>
-      <c r="I155" s="36"/>
-      <c r="J155" s="36"/>
-      <c r="K155" s="25"/>
+      <c r="A155" s="1"/>
+      <c r="B155" s="2"/>
+      <c r="C155" s="1"/>
+      <c r="D155" s="1"/>
+      <c r="E155" s="1"/>
+      <c r="F155" s="1"/>
+      <c r="G155" s="1"/>
+      <c r="H155" s="1"/>
+      <c r="I155" s="1"/>
+      <c r="J155" s="1"/>
+      <c r="K155" s="1"/>
       <c r="L155" s="1"/>
       <c r="M155" s="1"/>
       <c r="N155" s="1"/>
@@ -6601,17 +6543,17 @@
       <c r="Z155" s="1"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="A156" s="26"/>
-      <c r="B156" s="34"/>
-      <c r="C156" s="34"/>
-      <c r="D156" s="34"/>
-      <c r="E156" s="34"/>
-      <c r="F156" s="35"/>
-      <c r="G156" s="36"/>
-      <c r="H156" s="36"/>
-      <c r="I156" s="36"/>
-      <c r="J156" s="36"/>
-      <c r="K156" s="25"/>
+      <c r="A156" s="1"/>
+      <c r="B156" s="2"/>
+      <c r="C156" s="1"/>
+      <c r="D156" s="1"/>
+      <c r="E156" s="1"/>
+      <c r="F156" s="1"/>
+      <c r="G156" s="1"/>
+      <c r="H156" s="1"/>
+      <c r="I156" s="1"/>
+      <c r="J156" s="1"/>
+      <c r="K156" s="1"/>
       <c r="L156" s="1"/>
       <c r="M156" s="1"/>
       <c r="N156" s="1"/>
@@ -6629,17 +6571,17 @@
       <c r="Z156" s="1"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="A157" s="26"/>
-      <c r="B157" s="37"/>
-      <c r="C157" s="37"/>
-      <c r="D157" s="37"/>
-      <c r="E157" s="37"/>
-      <c r="F157" s="35"/>
-      <c r="G157" s="36"/>
-      <c r="H157" s="36"/>
-      <c r="I157" s="36"/>
-      <c r="J157" s="36"/>
-      <c r="K157" s="25"/>
+      <c r="A157" s="1"/>
+      <c r="B157" s="2"/>
+      <c r="C157" s="1"/>
+      <c r="D157" s="1"/>
+      <c r="E157" s="1"/>
+      <c r="F157" s="1"/>
+      <c r="G157" s="1"/>
+      <c r="H157" s="1"/>
+      <c r="I157" s="1"/>
+      <c r="J157" s="1"/>
+      <c r="K157" s="1"/>
       <c r="L157" s="1"/>
       <c r="M157" s="1"/>
       <c r="N157" s="1"/>
@@ -6657,17 +6599,17 @@
       <c r="Z157" s="1"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="A158" s="26"/>
-      <c r="B158" s="38"/>
-      <c r="C158" s="36"/>
-      <c r="D158" s="36"/>
-      <c r="E158" s="36"/>
-      <c r="F158" s="35"/>
-      <c r="G158" s="36"/>
-      <c r="H158" s="36"/>
-      <c r="I158" s="36"/>
-      <c r="J158" s="36"/>
-      <c r="K158" s="25"/>
+      <c r="A158" s="1"/>
+      <c r="B158" s="2"/>
+      <c r="C158" s="1"/>
+      <c r="D158" s="1"/>
+      <c r="E158" s="1"/>
+      <c r="F158" s="1"/>
+      <c r="G158" s="1"/>
+      <c r="H158" s="1"/>
+      <c r="I158" s="1"/>
+      <c r="J158" s="1"/>
+      <c r="K158" s="1"/>
       <c r="L158" s="1"/>
       <c r="M158" s="1"/>
       <c r="N158" s="1"/>
@@ -6686,15 +6628,15 @@
     </row>
     <row r="159" ht="15.75" customHeight="1">
       <c r="A159" s="1"/>
-      <c r="B159" s="39"/>
-      <c r="C159" s="40"/>
-      <c r="D159" s="40"/>
-      <c r="E159" s="40"/>
-      <c r="F159" s="40"/>
-      <c r="G159" s="40"/>
-      <c r="H159" s="40"/>
-      <c r="I159" s="40"/>
-      <c r="J159" s="40"/>
+      <c r="B159" s="2"/>
+      <c r="C159" s="1"/>
+      <c r="D159" s="1"/>
+      <c r="E159" s="1"/>
+      <c r="F159" s="1"/>
+      <c r="G159" s="1"/>
+      <c r="H159" s="1"/>
+      <c r="I159" s="1"/>
+      <c r="J159" s="1"/>
       <c r="K159" s="1"/>
       <c r="L159" s="1"/>
       <c r="M159" s="1"/>
@@ -30120,148 +30062,8 @@
       <c r="Y995" s="1"/>
       <c r="Z995" s="1"/>
     </row>
-    <row r="996" ht="15.75" customHeight="1">
-      <c r="A996" s="1"/>
-      <c r="B996" s="2"/>
-      <c r="C996" s="1"/>
-      <c r="D996" s="1"/>
-      <c r="E996" s="1"/>
-      <c r="F996" s="1"/>
-      <c r="G996" s="1"/>
-      <c r="H996" s="1"/>
-      <c r="I996" s="1"/>
-      <c r="J996" s="1"/>
-      <c r="K996" s="1"/>
-      <c r="L996" s="1"/>
-      <c r="M996" s="1"/>
-      <c r="N996" s="1"/>
-      <c r="O996" s="1"/>
-      <c r="P996" s="1"/>
-      <c r="Q996" s="1"/>
-      <c r="R996" s="1"/>
-      <c r="S996" s="1"/>
-      <c r="T996" s="1"/>
-      <c r="U996" s="1"/>
-      <c r="V996" s="1"/>
-      <c r="W996" s="1"/>
-      <c r="X996" s="1"/>
-      <c r="Y996" s="1"/>
-      <c r="Z996" s="1"/>
-    </row>
-    <row r="997" ht="15.75" customHeight="1">
-      <c r="A997" s="1"/>
-      <c r="B997" s="2"/>
-      <c r="C997" s="1"/>
-      <c r="D997" s="1"/>
-      <c r="E997" s="1"/>
-      <c r="F997" s="1"/>
-      <c r="G997" s="1"/>
-      <c r="H997" s="1"/>
-      <c r="I997" s="1"/>
-      <c r="J997" s="1"/>
-      <c r="K997" s="1"/>
-      <c r="L997" s="1"/>
-      <c r="M997" s="1"/>
-      <c r="N997" s="1"/>
-      <c r="O997" s="1"/>
-      <c r="P997" s="1"/>
-      <c r="Q997" s="1"/>
-      <c r="R997" s="1"/>
-      <c r="S997" s="1"/>
-      <c r="T997" s="1"/>
-      <c r="U997" s="1"/>
-      <c r="V997" s="1"/>
-      <c r="W997" s="1"/>
-      <c r="X997" s="1"/>
-      <c r="Y997" s="1"/>
-      <c r="Z997" s="1"/>
-    </row>
-    <row r="998" ht="15.75" customHeight="1">
-      <c r="A998" s="1"/>
-      <c r="B998" s="2"/>
-      <c r="C998" s="1"/>
-      <c r="D998" s="1"/>
-      <c r="E998" s="1"/>
-      <c r="F998" s="1"/>
-      <c r="G998" s="1"/>
-      <c r="H998" s="1"/>
-      <c r="I998" s="1"/>
-      <c r="J998" s="1"/>
-      <c r="K998" s="1"/>
-      <c r="L998" s="1"/>
-      <c r="M998" s="1"/>
-      <c r="N998" s="1"/>
-      <c r="O998" s="1"/>
-      <c r="P998" s="1"/>
-      <c r="Q998" s="1"/>
-      <c r="R998" s="1"/>
-      <c r="S998" s="1"/>
-      <c r="T998" s="1"/>
-      <c r="U998" s="1"/>
-      <c r="V998" s="1"/>
-      <c r="W998" s="1"/>
-      <c r="X998" s="1"/>
-      <c r="Y998" s="1"/>
-      <c r="Z998" s="1"/>
-    </row>
-    <row r="999" ht="15.75" customHeight="1">
-      <c r="A999" s="1"/>
-      <c r="B999" s="2"/>
-      <c r="C999" s="1"/>
-      <c r="D999" s="1"/>
-      <c r="E999" s="1"/>
-      <c r="F999" s="1"/>
-      <c r="G999" s="1"/>
-      <c r="H999" s="1"/>
-      <c r="I999" s="1"/>
-      <c r="J999" s="1"/>
-      <c r="K999" s="1"/>
-      <c r="L999" s="1"/>
-      <c r="M999" s="1"/>
-      <c r="N999" s="1"/>
-      <c r="O999" s="1"/>
-      <c r="P999" s="1"/>
-      <c r="Q999" s="1"/>
-      <c r="R999" s="1"/>
-      <c r="S999" s="1"/>
-      <c r="T999" s="1"/>
-      <c r="U999" s="1"/>
-      <c r="V999" s="1"/>
-      <c r="W999" s="1"/>
-      <c r="X999" s="1"/>
-      <c r="Y999" s="1"/>
-      <c r="Z999" s="1"/>
-    </row>
-    <row r="1000" ht="15.75" customHeight="1">
-      <c r="A1000" s="1"/>
-      <c r="B1000" s="2"/>
-      <c r="C1000" s="1"/>
-      <c r="D1000" s="1"/>
-      <c r="E1000" s="1"/>
-      <c r="F1000" s="1"/>
-      <c r="G1000" s="1"/>
-      <c r="H1000" s="1"/>
-      <c r="I1000" s="1"/>
-      <c r="J1000" s="1"/>
-      <c r="K1000" s="1"/>
-      <c r="L1000" s="1"/>
-      <c r="M1000" s="1"/>
-      <c r="N1000" s="1"/>
-      <c r="O1000" s="1"/>
-      <c r="P1000" s="1"/>
-      <c r="Q1000" s="1"/>
-      <c r="R1000" s="1"/>
-      <c r="S1000" s="1"/>
-      <c r="T1000" s="1"/>
-      <c r="U1000" s="1"/>
-      <c r="V1000" s="1"/>
-      <c r="W1000" s="1"/>
-      <c r="X1000" s="1"/>
-      <c r="Y1000" s="1"/>
-      <c r="Z1000" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="271">
+  <mergeCells count="262">
     <mergeCell ref="G4:G7"/>
     <mergeCell ref="H4:H7"/>
     <mergeCell ref="I4:I7"/>
@@ -30327,44 +30129,35 @@
     <mergeCell ref="F55:F57"/>
     <mergeCell ref="G55:G57"/>
     <mergeCell ref="H55:H57"/>
-    <mergeCell ref="I60:I62"/>
-    <mergeCell ref="J60:J62"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="C59:C62"/>
-    <mergeCell ref="D59:D62"/>
-    <mergeCell ref="E59:E62"/>
-    <mergeCell ref="F60:F62"/>
-    <mergeCell ref="G60:G62"/>
-    <mergeCell ref="H60:H62"/>
-    <mergeCell ref="B94:B97"/>
-    <mergeCell ref="C94:C97"/>
-    <mergeCell ref="D94:D97"/>
-    <mergeCell ref="E94:E97"/>
-    <mergeCell ref="F95:F97"/>
-    <mergeCell ref="G95:G97"/>
-    <mergeCell ref="H95:H97"/>
-    <mergeCell ref="I95:I97"/>
-    <mergeCell ref="J95:J97"/>
-    <mergeCell ref="F80:F82"/>
-    <mergeCell ref="G80:G82"/>
-    <mergeCell ref="H80:H82"/>
-    <mergeCell ref="I80:I82"/>
-    <mergeCell ref="J80:J82"/>
-    <mergeCell ref="H70:H72"/>
-    <mergeCell ref="I70:I72"/>
-    <mergeCell ref="F70:F72"/>
-    <mergeCell ref="F65:F67"/>
-    <mergeCell ref="G65:G67"/>
-    <mergeCell ref="H65:H67"/>
-    <mergeCell ref="I65:I67"/>
-    <mergeCell ref="J65:J67"/>
+    <mergeCell ref="B89:B92"/>
+    <mergeCell ref="C89:C92"/>
+    <mergeCell ref="D89:D92"/>
+    <mergeCell ref="E89:E92"/>
+    <mergeCell ref="F90:F92"/>
+    <mergeCell ref="G90:G92"/>
+    <mergeCell ref="H90:H92"/>
+    <mergeCell ref="I90:I92"/>
+    <mergeCell ref="J90:J92"/>
     <mergeCell ref="F75:F77"/>
     <mergeCell ref="G75:G77"/>
     <mergeCell ref="H75:H77"/>
     <mergeCell ref="I75:I77"/>
     <mergeCell ref="J75:J77"/>
+    <mergeCell ref="H65:H67"/>
+    <mergeCell ref="I65:I67"/>
+    <mergeCell ref="F65:F67"/>
+    <mergeCell ref="F60:F62"/>
+    <mergeCell ref="G60:G62"/>
+    <mergeCell ref="H60:H62"/>
+    <mergeCell ref="I60:I62"/>
+    <mergeCell ref="J60:J62"/>
+    <mergeCell ref="F70:F72"/>
     <mergeCell ref="G70:G72"/>
+    <mergeCell ref="H70:H72"/>
+    <mergeCell ref="I70:I72"/>
     <mergeCell ref="J70:J72"/>
+    <mergeCell ref="G65:G67"/>
+    <mergeCell ref="J65:J67"/>
     <mergeCell ref="I19:I22"/>
     <mergeCell ref="J19:J22"/>
     <mergeCell ref="B19:B22"/>
@@ -30396,8 +30189,17 @@
     <mergeCell ref="B34:B37"/>
     <mergeCell ref="C34:C37"/>
     <mergeCell ref="D34:D37"/>
-    <mergeCell ref="D79:D82"/>
-    <mergeCell ref="E79:E82"/>
+    <mergeCell ref="D74:D77"/>
+    <mergeCell ref="E74:E77"/>
+    <mergeCell ref="I130:I132"/>
+    <mergeCell ref="J130:J132"/>
+    <mergeCell ref="B129:B132"/>
+    <mergeCell ref="D129:D132"/>
+    <mergeCell ref="E129:E132"/>
+    <mergeCell ref="F130:F132"/>
+    <mergeCell ref="G130:G132"/>
+    <mergeCell ref="H130:H132"/>
+    <mergeCell ref="C129:C132"/>
     <mergeCell ref="I135:I137"/>
     <mergeCell ref="J135:J137"/>
     <mergeCell ref="B134:B137"/>
@@ -30407,14 +30209,14 @@
     <mergeCell ref="G135:G137"/>
     <mergeCell ref="H135:H137"/>
     <mergeCell ref="C134:C137"/>
-    <mergeCell ref="I140:I142"/>
-    <mergeCell ref="J140:J142"/>
+    <mergeCell ref="I139:I142"/>
+    <mergeCell ref="J139:J142"/>
     <mergeCell ref="B139:B142"/>
     <mergeCell ref="D139:D142"/>
     <mergeCell ref="E139:E142"/>
-    <mergeCell ref="F140:F142"/>
-    <mergeCell ref="G140:G142"/>
-    <mergeCell ref="H140:H142"/>
+    <mergeCell ref="F139:F142"/>
+    <mergeCell ref="G139:G142"/>
+    <mergeCell ref="H139:H142"/>
     <mergeCell ref="C139:C142"/>
     <mergeCell ref="I144:I147"/>
     <mergeCell ref="J144:J147"/>
@@ -30425,72 +30227,72 @@
     <mergeCell ref="G144:G147"/>
     <mergeCell ref="H144:H147"/>
     <mergeCell ref="C144:C147"/>
-    <mergeCell ref="I149:I152"/>
-    <mergeCell ref="J149:J152"/>
-    <mergeCell ref="B149:B152"/>
-    <mergeCell ref="D149:D152"/>
-    <mergeCell ref="E149:E152"/>
-    <mergeCell ref="F149:F152"/>
-    <mergeCell ref="G149:G152"/>
-    <mergeCell ref="H149:H152"/>
-    <mergeCell ref="C149:C152"/>
-    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="C59:C62"/>
+    <mergeCell ref="D59:D62"/>
+    <mergeCell ref="E59:E62"/>
     <mergeCell ref="C64:C67"/>
     <mergeCell ref="D64:D67"/>
     <mergeCell ref="E64:E67"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="B69:B72"/>
     <mergeCell ref="C69:C72"/>
     <mergeCell ref="D69:D72"/>
     <mergeCell ref="E69:E72"/>
-    <mergeCell ref="B69:B72"/>
     <mergeCell ref="B74:B77"/>
     <mergeCell ref="C74:C77"/>
-    <mergeCell ref="D74:D77"/>
-    <mergeCell ref="E74:E77"/>
+    <mergeCell ref="I80:I82"/>
+    <mergeCell ref="J80:J82"/>
     <mergeCell ref="B79:B82"/>
     <mergeCell ref="C79:C82"/>
-    <mergeCell ref="I85:I87"/>
-    <mergeCell ref="J85:J87"/>
+    <mergeCell ref="D79:D82"/>
+    <mergeCell ref="E79:E82"/>
+    <mergeCell ref="F80:F82"/>
+    <mergeCell ref="G80:G82"/>
+    <mergeCell ref="H80:H82"/>
+    <mergeCell ref="I84:I87"/>
+    <mergeCell ref="J84:J87"/>
     <mergeCell ref="B84:B87"/>
     <mergeCell ref="C84:C87"/>
     <mergeCell ref="D84:D87"/>
     <mergeCell ref="E84:E87"/>
-    <mergeCell ref="F85:F87"/>
-    <mergeCell ref="G85:G87"/>
-    <mergeCell ref="H85:H87"/>
-    <mergeCell ref="I89:I92"/>
-    <mergeCell ref="J89:J92"/>
-    <mergeCell ref="B89:B92"/>
-    <mergeCell ref="C89:C92"/>
-    <mergeCell ref="D89:D92"/>
-    <mergeCell ref="E89:E92"/>
-    <mergeCell ref="F89:F92"/>
-    <mergeCell ref="G89:G92"/>
-    <mergeCell ref="H89:H92"/>
-    <mergeCell ref="B154:B157"/>
-    <mergeCell ref="C154:C157"/>
-    <mergeCell ref="D154:D157"/>
-    <mergeCell ref="E154:E157"/>
+    <mergeCell ref="F84:F87"/>
+    <mergeCell ref="G84:G87"/>
+    <mergeCell ref="H84:H87"/>
+    <mergeCell ref="B149:B152"/>
+    <mergeCell ref="C149:C152"/>
+    <mergeCell ref="D149:D152"/>
+    <mergeCell ref="E149:E152"/>
+    <mergeCell ref="C114:C117"/>
     <mergeCell ref="C119:C122"/>
     <mergeCell ref="C124:C127"/>
-    <mergeCell ref="C129:C132"/>
-    <mergeCell ref="I99:I102"/>
-    <mergeCell ref="J99:J102"/>
+    <mergeCell ref="I94:I97"/>
+    <mergeCell ref="J94:J97"/>
+    <mergeCell ref="B94:B97"/>
+    <mergeCell ref="C94:C97"/>
+    <mergeCell ref="D94:D97"/>
+    <mergeCell ref="E94:E97"/>
+    <mergeCell ref="F94:F97"/>
+    <mergeCell ref="G94:G97"/>
+    <mergeCell ref="H94:H97"/>
+    <mergeCell ref="I100:I102"/>
+    <mergeCell ref="J100:J102"/>
     <mergeCell ref="B99:B102"/>
     <mergeCell ref="C99:C102"/>
     <mergeCell ref="D99:D102"/>
     <mergeCell ref="E99:E102"/>
-    <mergeCell ref="F99:F102"/>
-    <mergeCell ref="G99:G102"/>
-    <mergeCell ref="H99:H102"/>
-    <mergeCell ref="I105:I107"/>
-    <mergeCell ref="J105:J107"/>
+    <mergeCell ref="F100:F102"/>
+    <mergeCell ref="G100:G102"/>
+    <mergeCell ref="H100:H102"/>
+    <mergeCell ref="I104:I107"/>
+    <mergeCell ref="J104:J107"/>
     <mergeCell ref="B104:B107"/>
     <mergeCell ref="C104:C107"/>
     <mergeCell ref="D104:D107"/>
     <mergeCell ref="E104:E107"/>
-    <mergeCell ref="F105:F107"/>
-    <mergeCell ref="G105:G107"/>
-    <mergeCell ref="H105:H107"/>
+    <mergeCell ref="F104:F107"/>
+    <mergeCell ref="G104:G107"/>
+    <mergeCell ref="H104:H107"/>
     <mergeCell ref="I109:I112"/>
     <mergeCell ref="J109:J112"/>
     <mergeCell ref="B109:B112"/>
@@ -30503,7 +30305,6 @@
     <mergeCell ref="I114:I117"/>
     <mergeCell ref="J114:J117"/>
     <mergeCell ref="B114:B117"/>
-    <mergeCell ref="C114:C117"/>
     <mergeCell ref="D114:D117"/>
     <mergeCell ref="E114:E117"/>
     <mergeCell ref="F114:F117"/>
@@ -30517,22 +30318,14 @@
     <mergeCell ref="F119:F122"/>
     <mergeCell ref="G119:G122"/>
     <mergeCell ref="H119:H122"/>
-    <mergeCell ref="I124:I127"/>
-    <mergeCell ref="J124:J127"/>
+    <mergeCell ref="I125:I127"/>
+    <mergeCell ref="J125:J127"/>
     <mergeCell ref="B124:B127"/>
     <mergeCell ref="D124:D127"/>
     <mergeCell ref="E124:E127"/>
-    <mergeCell ref="F124:F127"/>
-    <mergeCell ref="G124:G127"/>
-    <mergeCell ref="H124:H127"/>
-    <mergeCell ref="I130:I132"/>
-    <mergeCell ref="J130:J132"/>
-    <mergeCell ref="B129:B132"/>
-    <mergeCell ref="D129:D132"/>
-    <mergeCell ref="E129:E132"/>
-    <mergeCell ref="F130:F132"/>
-    <mergeCell ref="G130:G132"/>
-    <mergeCell ref="H130:H132"/>
+    <mergeCell ref="F125:F127"/>
+    <mergeCell ref="G125:G127"/>
+    <mergeCell ref="H125:H127"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>